<commit_message>
fixed inputs for power plants
</commit_message>
<xml_diff>
--- a/data/Datamaps.xlsx
+++ b/data/Datamaps.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B9D058-2FCF-4748-A085-AA6E04C7A6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F216C7B-5260-40D0-92CB-31A8B50D8515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6C87355B-11EA-46CA-BA02-93BC4926DC2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="from traderes to emlab" sheetId="2" r:id="rId2"/>
+    <sheet name="data per year" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>emlab</t>
   </si>
@@ -149,6 +149,51 @@
   </si>
   <si>
     <t>save loan in power plant</t>
+  </si>
+  <si>
+    <t>MarketClearingPoints</t>
+  </si>
+  <si>
+    <t>MarketClearingPoint 2021-08-04 13:27:00.769896</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>CO2Auction</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>TotalCapacity</t>
+  </si>
+  <si>
+    <t>PowerPlants</t>
+  </si>
+  <si>
+    <t>SunPV</t>
+  </si>
+  <si>
+    <t>MWNL</t>
+  </si>
+  <si>
+    <t>12291,7</t>
+  </si>
+  <si>
+    <t>WindOff</t>
+  </si>
+  <si>
+    <t>WindOn</t>
+  </si>
+  <si>
+    <t>SystemClockTicks</t>
+  </si>
+  <si>
+    <t>ticks</t>
+  </si>
+  <si>
+    <t>data per year in competes-emlab emlab</t>
   </si>
 </sst>
 </file>
@@ -558,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2B93C7-EA7D-47DD-B6A1-A4A1424F5FD3}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -589,7 +634,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -597,7 +642,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -780,15 +825,145 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8432F7E-C15C-49B4-B6CB-7FC76C88BCCC}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320171F4-F369-42DB-9E7C-B47E7F64F920}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" customWidth="1"/>
+    <col min="2" max="2" width="33.08984375" customWidth="1"/>
+    <col min="3" max="5" width="23.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
write conventionals for amiris excel
</commit_message>
<xml_diff>
--- a/data/Datamaps.xlsx
+++ b/data/Datamaps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FD170C-573B-41FE-82FC-072529C9CB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5C9E78-D49D-4DB3-9DFA-0A77AEE08846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6C87355B-11EA-46CA-BA02-93BC4926DC2A}"/>
+    <workbookView xWindow="-5550" yWindow="-21720" windowWidth="37710" windowHeight="21840" activeTab="1" xr2:uid="{6C87355B-11EA-46CA-BA02-93BC4926DC2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
   <si>
     <t>emlab</t>
   </si>
@@ -144,15 +144,6 @@
   </si>
   <si>
     <t>calculated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">create cash flow </t>
-  </si>
-  <si>
-    <t>create loan and assign loan to power plant</t>
-  </si>
-  <si>
-    <t>save loan in power plant</t>
   </si>
   <si>
     <t>MarketClearingPoints</t>
@@ -753,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2B93C7-EA7D-47DD-B6A1-A4A1424F5FD3}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="A23" sqref="A23:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -952,21 +943,6 @@
       </c>
       <c r="B22" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -981,41 +957,42 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.08984375" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" customWidth="1"/>
     <col min="8" max="8" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
         <v>78</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C2">
         <v>0.20448</v>
@@ -1027,25 +1004,25 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5">
         <v>0.26388</v>
@@ -1057,20 +1034,20 @@
         <v>0.5</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <v>0.34</v>
@@ -1082,25 +1059,25 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10">
         <v>0.26750000000000002</v>
@@ -1112,15 +1089,15 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C11">
         <v>0.41</v>
@@ -1132,15 +1109,15 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C12">
         <v>0.20448</v>
@@ -1152,15 +1129,15 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1172,25 +1149,25 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
         <v>67</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1202,12 +1179,12 @@
         <v>0.5</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17">
         <v>0.20448</v>
@@ -1219,12 +1196,12 @@
         <v>0.5</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1236,12 +1213,12 @@
         <v>0.5</v>
       </c>
       <c r="F18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1253,12 +1230,12 @@
         <v>0.5</v>
       </c>
       <c r="F19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1270,12 +1247,12 @@
         <v>0.5</v>
       </c>
       <c r="F20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1287,12 +1264,12 @@
         <v>0.5</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1304,12 +1281,12 @@
         <v>0.5</v>
       </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1321,12 +1298,12 @@
         <v>0.5</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1338,7 +1315,7 @@
         <v>0.5</v>
       </c>
       <c r="F24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1363,30 +1340,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1397,13 +1374,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1414,30 +1391,30 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1448,13 +1425,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1465,13 +1442,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1482,7 +1459,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>